<commit_message>
- add table about sequence
git-svn-id: file:///E/Local_Repository/Asset_Health/trunk@25 9a2719d2-1c2b-0a45-af5b-2640030c331b
</commit_message>
<xml_diff>
--- a/TableBuilder/xlsx_Data/MessageTable.xlsx
+++ b/TableBuilder/xlsx_Data/MessageTable.xlsx
@@ -159,9 +159,6 @@
     <t>AskHelp2</t>
   </si>
   <si>
-    <t>What can I help for you?</t>
-  </si>
-  <si>
     <t>StrHelp</t>
   </si>
   <si>
@@ -249,9 +246,6 @@
     <t>speak</t>
   </si>
   <si>
-    <t>Hello {0}.</t>
-  </si>
-  <si>
     <t>!Enum:eGroupTag</t>
   </si>
   <si>
@@ -322,6 +316,12 @@
   </si>
   <si>
     <t>elseCase</t>
+  </si>
+  <si>
+    <t>Hello {0}. | What's up? {0} | What's going on? {0}</t>
+  </si>
+  <si>
+    <t>What can I help you?</t>
   </si>
 </sst>
 </file>
@@ -948,7 +948,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -977,16 +977,16 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
@@ -1017,18 +1017,18 @@
     </row>
     <row r="4" spans="1:7" ht="17.399999999999999">
       <c r="A4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1041,10 +1041,10 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="5"/>
     </row>
@@ -1058,7 +1058,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="1"/>
@@ -1068,12 +1068,12 @@
         <v>42</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -1087,7 +1087,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="1"/>
@@ -1102,7 +1102,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>
@@ -1117,7 +1117,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="1"/>
@@ -1132,7 +1132,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="1"/>
@@ -1147,16 +1147,16 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="17.399999999999999">
       <c r="A13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1182,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1200,29 +1200,29 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="17.399999999999999">
       <c r="A2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>1</v>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="3" spans="1:6" ht="17.399999999999999">
       <c r="A3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -1256,13 +1256,13 @@
         <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>11</v>
@@ -1288,63 +1288,15 @@
       <c r="E6" s="5"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="17.399999999999999">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" ht="17.399999999999999">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="17.399999999999999">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="17.399999999999999">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="17.399999999999999">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="17.399999999999999">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1356,7 +1308,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1380,22 +1332,22 @@
     </row>
     <row r="2" spans="1:11" ht="17.399999999999999">
       <c r="A2" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
@@ -1404,12 +1356,12 @@
         <v>5</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="17.399999999999999">
       <c r="A3" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -1424,13 +1376,13 @@
         <v>4</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>4</v>
@@ -1438,74 +1390,74 @@
     </row>
     <row r="4" spans="1:11" ht="17.399999999999999">
       <c r="A4" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17.399999999999999">
       <c r="A5" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="17.399999999999999">
       <c r="A6" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>13</v>
@@ -1513,20 +1465,20 @@
     </row>
     <row r="7" spans="1:11" ht="17.399999999999999">
       <c r="A7" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>21</v>
@@ -1534,68 +1486,68 @@
     </row>
     <row r="8" spans="1:11" ht="17.399999999999999">
       <c r="A8" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="17.399999999999999">
       <c r="A9" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G9" s="1"/>
       <c r="J9" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="17.399999999999999">
       <c r="A10" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="G10" s="1"/>
       <c r="J10" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1609,7 +1561,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="1"/>
       <c r="J11" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="17.399999999999999">
@@ -1621,18 +1573,18 @@
       <c r="F12" s="5"/>
       <c r="G12" s="1"/>
       <c r="J12" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="G13" s="1"/>
       <c r="J13" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="J14" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>